<commit_message>
table res done  okey
</commit_message>
<xml_diff>
--- a/src/utils/req-res.xlsx
+++ b/src/utils/req-res.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sveshnikova\Desktop\anc\dev\stand_modeling\src\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Елена\Desktop\dev\stend_modeling\src\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63BF81C-9167-493E-9672-62193E6CCAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3C8661-4E80-4AF0-A14A-610A1B479996}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A351F8E5-E25F-43C0-BCFC-9311EC29C128}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A351F8E5-E25F-43C0-BCFC-9311EC29C128}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>описание</t>
   </si>
@@ -39,9 +39,6 @@
     <t>http://modeller:9090/modelling_result_list</t>
   </si>
   <si>
-    <t>{"success": 1, "configurations": {"0_2020-01-01-2020-01-02": {"instruments": [{"nsr": 10093, "cod": "Кис2", "locname": "Кисловодск", ...}]}, "1_2020-01-01-2020-01-02": {"instruments": [{"nsr": 10093, "cod": "Кис2", "locname": "Кисловодск", ...}, {"nsr": 10316, "cod": "Блг7", "locname": "Благовещенск",...}]}}}</t>
-  </si>
-  <si>
     <t>http://modeller:9090/modelling_result?id=0_2020-01-01-2020-01-02</t>
   </si>
   <si>
@@ -75,7 +72,103 @@
     <t>параметры(get) или тело запроса(post)</t>
   </si>
   <si>
-    <t>{"success": 1, "min size inc height": {"type": "image", "data": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAA"}, min_size_inc_height: {type: 'image', data: 'data:image/png;base64,iVBOR"}}</t>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>http://modeller:9090/run_modelling</t>
+  </si>
+  <si>
+    <t>{"success":1,"message":"running process 1"}</t>
+  </si>
+  <si>
+    <t>{
+ "start_date":"2020-01-01",
+ "end_date":"2020-12-31",
+ "catalogue":"2020",
+ "instruments": [
+   {
+  "nsr": 10093,
+  "cod": "Кис2",
+  "locname":"Кисловодск",
+  "latitude": 43.7402600307874,
+  "longitude": 42.6536598478286,
+  "altitude": 2107.7471803287,
+  "aperture": 19.2,
+  "secondary_coefficient": 0.52,
+  "pixel_scale": 6.3,
+  "readout_noise":5,
+  "fovx": 14.0,
+  "fovy": 9.0,
+  "frame_readout": 0.5,
+  "frame_flush": 5.0,
+  "task_switch_time": 6,
+  "stabilization_time": 10,
+  "mount_type":"экваториальная",
+  "slew_vel_alpha": 1.8,
+  "slew_vel_delta": 1.8,
+  "min_elevation": 10,
+  "transmittivity": 0.5,
+  "quantum_efficiency": 0.8,
+  "mode": "обзор",
+  "noko_twilight": false,
+  "noko": false,
+  "gso_survey": true
+   }
+ ],
+ "sun_elevation":18,
+ "detectable_snr":3.0,
+ "max_exp":7.0,
+ "max_track_length":0.05,
+ "zenith_sky_brightness":22
+  }</t>
+  </si>
+  <si>
+    <t>{
+  "success": 1,
+  "min size inc height": {
+    "type": "image",
+    "data": "data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAA"
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  "success": 1,
+  "configurations": {
+    "0_2020-01-01-2020-01-02": {
+      "instruments": [
+        {
+          "nsr": 10093,
+          "cod": "Кис2",
+          "locname": "Кисловодск",
+          "latitude": 43.7402600307874,
+          "longitude": 42.6536598478286,
+          "altitude": 2107.7471803287,
+          "aperture": 19.2,
+          "secondary_coefficient": 0.52,
+          "pixel_scale": 6.3,
+          "readout_noise": 5,
+          "fovx": 14.0,
+          "fovy": 9.0,
+          "frame_readout": 0.5,
+          "frame_flush": 5.0,
+          "task_switch_time": 6,
+          "stabilization_time": 10,
+          "mount_type": "экваториальная",
+          "slew_vel_alpha": 1.8,
+          "slew_vel_delta": 1.8,
+          "min_elevation": 10,
+          "transmittivity": 0.5,
+          "quantum_efficiency": 0.8,
+          "mode": "обзор",
+          "noko_twilight": false,
+          "noko": false,
+          "gso_survey": true
+        }
+      ]
+    }
+  }
+}</t>
   </si>
 </sst>
 </file>
@@ -177,22 +270,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6820E0BF-F5DB-4BFA-AAB1-8C862B2381BA}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,117 +620,125 @@
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
     <col min="5" max="5" width="57.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>

</xml_diff>